<commit_message>
Prompting sesion 6 y 7
</commit_message>
<xml_diff>
--- a/Proyecto Final Desarrollo ABAP con COPILOT.xlsx
+++ b/Proyecto Final Desarrollo ABAP con COPILOT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwhid\Documents\GitHub\Curso-Github-Copilot\Jhonatan Hidalgo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwhid\Documents\GitHub\Proyecto_Copilot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDE2A886-A94F-4111-89B0-16F4EB9BE1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AC04C3-C049-4DB9-9ADE-62D6FE9E3EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="2820" windowWidth="23256" windowHeight="12456" xr2:uid="{90EE437F-81CB-4A4E-AE2C-0A8773015A8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90EE437F-81CB-4A4E-AE2C-0A8773015A8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C1BD49-78DA-4960-B5DA-5250E24FCA41}">
   <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +647,9 @@
       <c r="C6">
         <v>4</v>
       </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
@@ -658,6 +661,9 @@
       <c r="C7">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
@@ -669,6 +675,9 @@
       <c r="C8">
         <v>6</v>
       </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -680,6 +689,9 @@
       <c r="C9">
         <v>6</v>
       </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
@@ -691,6 +703,9 @@
       <c r="C10">
         <v>4</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
       <c r="E10" t="s">
         <v>19</v>
       </c>
@@ -705,7 +720,7 @@
       </c>
       <c r="D12">
         <f>SUM(D6:D10)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -930,7 +945,7 @@
       </c>
       <c r="D38">
         <f>SUM(D12,D20,D26,D32,D37)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -943,7 +958,7 @@
       </c>
       <c r="D39" s="5">
         <f>D38/40</f>
-        <v>0</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -956,7 +971,7 @@
       </c>
       <c r="D40" s="5">
         <f>D38/8</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Proyecto Final Desarrollo ABAP con COPILOT.xlsx
</commit_message>
<xml_diff>
--- a/Proyecto Final Desarrollo ABAP con COPILOT.xlsx
+++ b/Proyecto Final Desarrollo ABAP con COPILOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwhid\Documents\GitHub\Proyecto_Copilot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JhonatanHidalgo\Documents\GitHub\Proyecto_Copilot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93471EF3-29B5-464C-8F10-1B943FE16469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6991F9E9-C7B1-4E9D-ADEB-8D9235D01947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90EE437F-81CB-4A4E-AE2C-0A8773015A8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{90EE437F-81CB-4A4E-AE2C-0A8773015A8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Proyecto</t>
   </si>
@@ -601,30 +601,30 @@
   <dimension ref="B2:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="69.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
       <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
@@ -635,12 +635,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -654,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -668,7 +668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -682,7 +682,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -696,7 +696,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -710,7 +710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
@@ -723,66 +723,87 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
+      <c r="D15">
+        <v>2.5</v>
+      </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>28</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
+      <c r="D16">
+        <v>2.5</v>
+      </c>
       <c r="E16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>2.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
@@ -791,16 +812,16 @@
         <v>20</v>
       </c>
       <c r="D20">
-        <f>SUM(D15:D18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f>SUM(D15:D19)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -811,7 +832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -822,7 +843,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -833,7 +854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>32</v>
       </c>
@@ -844,7 +865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>5</v>
       </c>
@@ -857,12 +878,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -873,7 +894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -884,7 +905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -895,12 +916,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>5</v>
       </c>
@@ -913,12 +934,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -929,13 +950,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D37">
         <f>SUM(D35:D36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
@@ -945,10 +966,10 @@
       </c>
       <c r="D38">
         <f>SUM(D12,D20,D26,D32,D37)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
         <v>10</v>
       </c>
@@ -958,10 +979,10 @@
       </c>
       <c r="D39" s="5">
         <f>D38/40</f>
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
         <v>9</v>
       </c>
@@ -971,7 +992,7 @@
       </c>
       <c r="D40" s="5">
         <f>D38/8</f>
-        <v>1.875</v>
+        <v>3.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>